<commit_message>
actualizado de bot y puesta en marcha, asyncronia solucionada
</commit_message>
<xml_diff>
--- a/botwhats/src/Bot/chats/5491165188418@c.us.xlsx
+++ b/botwhats/src/Bot/chats/5491165188418@c.us.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>Fecha</t>
   </si>
@@ -108,6 +108,71 @@
   </si>
   <si>
     <t>*El instructor es de Buenos Aires, pero los cursos se dan en todo el pais.*</t>
+  </si>
+  <si>
+    <t>20-08-2021 01:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*🤖 Si le quedó una duda envieme un mensaje con algunos de las siguientes opciones para tener mas informacion*
+_Escriba a los números sin letras o números adicionales, luego envie el mensaje y le llegara la info que precisa._
+• Escriba la palabra *instructor* si desea hablar un tema en especifico con el instructor
+• Envie un *1* para saber cómo inscribirse de forma gratuita (sin certificado)
+• Envie un *2* para saber cómo inscribirse de forma paga (con certificado) y para saber cuando cuestan los certificados
+• Envie un *3* para saber cómo son los cursos, duración, pasos a seguir etc.
+• Envie un *4* para saber horarios del encuentro virtual de cada curso
+• Envie un *5* para saber de donde somos
+• Envie un *6* para saber si las clases son virtuales
+• Envie un *7* para saber cuanto tarda en llegar el certificado
+• Envie un *8* para ver modelos de certificados
+ *🤖 IMPORTANTE* si contesta algo diferente a lo de esta lista no podre responderle de manera adecuada. Recuerde que si desea hablar con el instructor debe enviar la palabra *instructor* como mensaje, yo me encargo de avisarle. 📬
+</t>
+  </si>
+  <si>
+    <t>20-08-2021 01:18</t>
+  </si>
+  <si>
+    <t>Hola Cin hermosa ❤. ¿Como estás?</t>
+  </si>
+  <si>
+    <t>20-08-2021 01:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🤖 *El instructor Ezequiel se contactará con usted cuando sea posible (estamos atendiendo muchas consultas)* ⏳ 
+_Mientras tanto puede consultarme a mi lo que desee_
+*Escriba el numero sin letras o números adicionales, luego envie el mensaje y le llegara la info que precisa.*
+• Envie un *1* para saber cómo inscribirse de forma gratuita (sin certificado)
+• Envie un *2* para saber cómo inscribirse de forma paga (con certificado) y para saber cuando cuestan los certificados
+• Envie un *3* para saber cómo son los cursos, duración, pasos a seguir etc.
+• Envie un *4* para saber horarios del encuentro virtual de cada curso
+• Envie un *5* para saber de donde somos
+• Envie un *6* para saber si las clases son virtuales
+• Envie un *7* para saber cuanto tarda en llegar el certificado
+• Envie un *8* para ver modelos de certificados
+    *🤖 IMPORTANTE* si contesta algo diferente a lo de esta lista no podre responderle de manera adecuada.
+    _El instructor se contactará a la brevedad_
+</t>
+  </si>
+  <si>
+    <t>20-08-2021 01:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*2) Inscripción paga (con certificado)*
+Debe abonar los certificados que desee y luego sumarse a los cursos
+*Modelos de Certificado* https://photos.app.goo.gl/Grm54bW161weeXB26
+*Promoción por pre-inscripción (hasta el lunes 23 inclusive)*
+• *Un (1)* Certificado *800$* https://mpago.la/2pwTDcY
+• *Dos (2)* Certificados *1000$* (500$ cada certificado)* ➤https://mpago.la/1noxX9Y
+• *Tres (3)* Certificados *1200$* (400$ cada certificado)* ➤https://mpago.la/2RKS4fA
+• *Cuatro (4)* Certificados *1400$* (350$ cada certificado)* ➤https://mpago.la/1eQvfze
+• *Cinco (5)* Certificados *1600$* (320$ cada certificado)* ➤https://mpago.la/234vbAd
+En total puede abonar hasta 5 certificados (porque son 5 cursos). Si abona menos de 5 certificados, deberá elegir en qué cursos utilizar el comprobante.
+*Luego de abonar debe unirse a los cursos que desee por los enlaces públicos de unión  https://docs.google.com/document/d/1H8DsbU-qfeIijVni4zrfG_ND1ugv_gNHq2x8dvFyiQU/edit?usp=sharing*
+*Formas de pago*
+• Débito
+• Crédito
+• Efectivo desde un Rapipago, Pago Facil, Kiosco o Provincia Net Pagos
+• Transferencias desde cuentas de mercado pago
+También puede abonarlos mediante una transferencia bancaria al 0140389103703753820095</t>
   </si>
 </sst>
 </file>
@@ -484,7 +549,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B23"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -623,6 +688,54 @@
         <v>10</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>